<commit_message>
Revert "Polymarket launch" revert This reverts commit 134c949c4800cf50d08eb2c40c89d7c918e3a9b0.
</commit_message>
<xml_diff>
--- a/logs/performance.xlsx
+++ b/logs/performance.xlsx
@@ -16,10 +16,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
-    <numFmt numFmtId="165" formatCode="YYYY-MM-DD"/>
-  </numFmts>
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -58,12 +55,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -429,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:P1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -519,56 +515,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="2" t="n">
-        <v>46027</v>
-      </c>
-      <c r="B2" t="n">
-        <v>6</v>
-      </c>
-      <c r="C2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" t="n">
-        <v>6</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" t="n">
-        <v>-0.411367454907323</v>
-      </c>
-      <c r="G2" t="n">
-        <v>-2.835595930727096</v>
-      </c>
-      <c r="H2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I2" t="n">
-        <v>0.06856124248455384</v>
-      </c>
-      <c r="J2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K2" t="n">
-        <v>-0.1000000000000001</v>
-      </c>
-      <c r="L2" t="n">
-        <v>0</v>
-      </c>
-      <c r="M2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N2" t="n">
-        <v>-65.3266029741873</v>
-      </c>
-      <c r="O2" t="n">
-        <v>316.4924961666666</v>
-      </c>
-      <c r="P2" t="n">
-        <v>28.63829188248484</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>